<commit_message>
Solucion del problema que teniamos
</commit_message>
<xml_diff>
--- a/Auxiliar.xlsx
+++ b/Auxiliar.xlsx
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -50,6 +50,27 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -425,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,14 +472,14 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>175204</t>
+          <t>175705</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>CDCDCF1</t>
+          <t>CDCDCO1</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -476,46 +497,492 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>CDCDCO2</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>2025-4</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>CDCDCS1</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>2025-4</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>CDCDMZ1</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>2025-4</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>CDCDRO1</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>2025-4</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="n"/>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>CDGD</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B22" s="1" t="inlineStr">
         <is>
           <t>2025-4</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>6010010007</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="n"/>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>CDSETSA</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>2025-4</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n"/>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
         <is>
           <t>CDVM</t>
         </is>
       </c>
-      <c r="B4" s="1" t="inlineStr">
+      <c r="B30" s="1" t="inlineStr">
         <is>
           <t>2025-4</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>6010010007</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n"/>
+      <c r="B31" s="1" t="n"/>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n"/>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>2026-1</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>6010010007</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n"/>
+      <c r="B33" s="1" t="n"/>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>6010010077</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B26:B27"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>